<commit_message>
Fixed burndown chart 3
Burndown chart 3 one of the day had 2 hours of work set but 3 hours were done, so it has been changed to 3 as the chart suggests
</commit_message>
<xml_diff>
--- a/docs/SprintBurndowns.xlsx
+++ b/docs/SprintBurndowns.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\computing\Desktop\SEGroup4\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Craig\Desktop\SEGroup4\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336143AD-F2E9-45DE-B5DD-06A233F4CA1A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="22185" yWindow="9750" windowWidth="24885" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -134,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,7 +273,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -633,7 +633,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -740,7 +739,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1101,7 +1099,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1208,7 +1205,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1309,28 +1305,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1407,28 +1403,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.285714285714286</c:v>
+                  <c:v>11.142857142857142</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.571428571428573</c:v>
+                  <c:v>9.2857142857142847</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8571428571428585</c:v>
+                  <c:v>7.428571428571427</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1428571428571441</c:v>
+                  <c:v>5.5714285714285694</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4285714285714297</c:v>
+                  <c:v>3.7142857142857122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7142857142857155</c:v>
+                  <c:v>1.857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-2.2204460492503131E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1569,7 +1565,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3679,11 +3674,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4954,7 +4949,7 @@
         <v>32</v>
       </c>
       <c r="E52" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -5125,35 +5120,35 @@
       </c>
       <c r="E60" s="1">
         <f>SUM(E49:E57)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" ref="F60:L60" si="2">E60-SUM(F49:F57)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G60" s="1">
         <f t="shared" si="2"/>
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
       <c r="H60" s="1">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J60" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K60" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
@@ -5168,35 +5163,35 @@
       </c>
       <c r="E61" s="1">
         <f>SUM(E49:E57)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F61" s="1">
         <f>E61-(E61/7)</f>
-        <v>10.285714285714286</v>
+        <v>11.142857142857142</v>
       </c>
       <c r="G61" s="1">
         <f>F61-(E61/7)</f>
-        <v>8.571428571428573</v>
+        <v>9.2857142857142847</v>
       </c>
       <c r="H61" s="1">
         <f>G61-(E61/7)</f>
-        <v>6.8571428571428585</v>
+        <v>7.428571428571427</v>
       </c>
       <c r="I61" s="1">
         <f>H61-(E61/7)</f>
-        <v>5.1428571428571441</v>
+        <v>5.5714285714285694</v>
       </c>
       <c r="J61" s="1">
         <f>I61-(E61/7)</f>
-        <v>3.4285714285714297</v>
+        <v>3.7142857142857122</v>
       </c>
       <c r="K61" s="1">
         <f>J61-(E61/7)</f>
-        <v>1.7142857142857155</v>
+        <v>1.857142857142855</v>
       </c>
       <c r="L61" s="1">
         <f>K61-(E61/7)</f>
-        <v>0</v>
+        <v>-2.2204460492503131E-15</v>
       </c>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>

</xml_diff>